<commit_message>
Moduling likehood and other functions
</commit_message>
<xml_diff>
--- a/TIMES.xlsx
+++ b/TIMES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3733C-075E-4CC5-85E9-7805F66AB142}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051AC38C-A076-411A-8E78-148E86B98BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Times" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="201">
   <si>
     <t>Número</t>
   </si>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>EMP</t>
+  </si>
+  <si>
+    <t>FUR</t>
   </si>
 </sst>
 </file>
@@ -872,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -894,9 +897,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G181" sqref="G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,13 +1253,13 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>1850</v>
       </c>
       <c r="E3" s="3">
@@ -1272,13 +1272,13 @@
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>1850</v>
       </c>
       <c r="E4" s="3">
@@ -1289,13 +1289,13 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>1850</v>
       </c>
       <c r="E5" s="3">
@@ -1306,13 +1306,13 @@
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>1850</v>
       </c>
       <c r="E6" s="3">
@@ -1323,13 +1323,13 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>1850</v>
       </c>
       <c r="E7" s="3">
@@ -1340,13 +1340,13 @@
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>1850</v>
       </c>
       <c r="E8" s="3">
@@ -1357,13 +1357,13 @@
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>1850</v>
       </c>
       <c r="E9" s="3">
@@ -1374,13 +1374,13 @@
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>1850</v>
       </c>
       <c r="E10" s="3">
@@ -1391,13 +1391,13 @@
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>1850</v>
       </c>
       <c r="E11" s="3">
@@ -1408,13 +1408,13 @@
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>1850</v>
       </c>
       <c r="E12" s="3">
@@ -1425,13 +1425,13 @@
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>1850</v>
       </c>
       <c r="E13" s="3">
@@ -1442,13 +1442,13 @@
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>1850</v>
       </c>
       <c r="E14" s="3">
@@ -1459,13 +1459,13 @@
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>1850</v>
       </c>
       <c r="E15" s="3">
@@ -1476,13 +1476,13 @@
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>1850</v>
       </c>
       <c r="E16" s="3">
@@ -1493,13 +1493,13 @@
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>1850</v>
       </c>
       <c r="E17" s="3">
@@ -1510,13 +1510,13 @@
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>1850</v>
       </c>
       <c r="E18" s="3">
@@ -1527,13 +1527,13 @@
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>1850</v>
       </c>
       <c r="E19" s="3">
@@ -1544,13 +1544,13 @@
       <c r="A20" s="17">
         <v>19</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>1850</v>
       </c>
       <c r="E20" s="3">
@@ -1561,13 +1561,13 @@
       <c r="A21" s="17">
         <v>20</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="21">
         <v>1800</v>
       </c>
       <c r="E21" s="3">
@@ -1578,13 +1578,13 @@
       <c r="A22" s="17">
         <v>21</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="21">
         <v>1800</v>
       </c>
       <c r="E22" s="3">
@@ -1595,13 +1595,13 @@
       <c r="A23" s="17">
         <v>22</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <v>1800</v>
       </c>
       <c r="E23" s="3">
@@ -1612,13 +1612,13 @@
       <c r="A24" s="17">
         <v>23</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="21">
         <v>1800</v>
       </c>
       <c r="E24" s="3">
@@ -1629,13 +1629,13 @@
       <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="21">
         <v>1800</v>
       </c>
       <c r="E25" s="3">
@@ -1646,13 +1646,13 @@
       <c r="A26" s="17">
         <v>25</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>1800</v>
       </c>
       <c r="E26" s="3">
@@ -1663,13 +1663,13 @@
       <c r="A27" s="17">
         <v>26</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="21">
         <v>1800</v>
       </c>
       <c r="E27" s="3">
@@ -1680,13 +1680,13 @@
       <c r="A28" s="17">
         <v>27</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="21">
         <v>1800</v>
       </c>
       <c r="E28" s="3">
@@ -1697,13 +1697,13 @@
       <c r="A29" s="17">
         <v>28</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="21">
         <v>1800</v>
       </c>
       <c r="E29" s="3">
@@ -1714,13 +1714,13 @@
       <c r="A30" s="17">
         <v>29</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="21">
         <v>1800</v>
       </c>
       <c r="E30" s="3">
@@ -1731,13 +1731,13 @@
       <c r="A31" s="17">
         <v>30</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="21">
         <v>1800</v>
       </c>
       <c r="E31" s="3">
@@ -1748,13 +1748,13 @@
       <c r="A32" s="17">
         <v>31</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="21">
         <v>1800</v>
       </c>
       <c r="E32" s="3">
@@ -1765,13 +1765,13 @@
       <c r="A33" s="17">
         <v>32</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="21">
         <v>1800</v>
       </c>
       <c r="E33" s="3">
@@ -1782,13 +1782,13 @@
       <c r="A34" s="17">
         <v>33</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="21">
         <v>1800</v>
       </c>
       <c r="E34" s="3">
@@ -1799,13 +1799,13 @@
       <c r="A35" s="17">
         <v>34</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="21">
         <v>1800</v>
       </c>
       <c r="E35" s="3">
@@ -1816,13 +1816,13 @@
       <c r="A36" s="17">
         <v>35</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="21">
         <v>1800</v>
       </c>
       <c r="E36" s="3">
@@ -1833,13 +1833,13 @@
       <c r="A37" s="17">
         <v>36</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="21">
         <v>1800</v>
       </c>
       <c r="E37" s="3">
@@ -1850,13 +1850,13 @@
       <c r="A38" s="17">
         <v>37</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="21">
         <v>1800</v>
       </c>
       <c r="E38" s="3">
@@ -1867,13 +1867,13 @@
       <c r="A39" s="17">
         <v>38</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="21">
         <v>1800</v>
       </c>
       <c r="E39" s="3">
@@ -1884,13 +1884,13 @@
       <c r="A40" s="17">
         <v>39</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="21">
         <v>1750</v>
       </c>
       <c r="E40" s="3">
@@ -1901,13 +1901,13 @@
       <c r="A41" s="17">
         <v>40</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="21">
         <v>1750</v>
       </c>
       <c r="E41" s="3">
@@ -1918,13 +1918,13 @@
       <c r="A42" s="17">
         <v>41</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="21">
         <v>1750</v>
       </c>
       <c r="E42" s="3">
@@ -1935,13 +1935,13 @@
       <c r="A43" s="17">
         <v>42</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="21">
         <v>1750</v>
       </c>
       <c r="E43" s="3">
@@ -1952,13 +1952,13 @@
       <c r="A44" s="17">
         <v>43</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="21">
         <v>1750</v>
       </c>
       <c r="E44" s="3">
@@ -1969,13 +1969,13 @@
       <c r="A45" s="17">
         <v>44</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="21">
         <v>1750</v>
       </c>
       <c r="E45" s="3">
@@ -1986,13 +1986,13 @@
       <c r="A46" s="17">
         <v>45</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="21">
         <v>1750</v>
       </c>
       <c r="E46" s="3">
@@ -2003,13 +2003,13 @@
       <c r="A47" s="17">
         <v>46</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="21">
         <v>1750</v>
       </c>
       <c r="E47" s="3">
@@ -2020,13 +2020,13 @@
       <c r="A48" s="17">
         <v>47</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="21">
         <v>1750</v>
       </c>
       <c r="E48" s="3">
@@ -2037,13 +2037,13 @@
       <c r="A49" s="17">
         <v>48</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="21">
         <v>1750</v>
       </c>
       <c r="E49" s="3">
@@ -2054,13 +2054,13 @@
       <c r="A50" s="17">
         <v>49</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="21">
         <v>1750</v>
       </c>
       <c r="E50" s="3">
@@ -2071,13 +2071,13 @@
       <c r="A51" s="17">
         <v>50</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="22">
+      <c r="D51" s="21">
         <v>1750</v>
       </c>
       <c r="E51" s="3">
@@ -2088,13 +2088,13 @@
       <c r="A52" s="17">
         <v>51</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="22">
+      <c r="D52" s="21">
         <v>1750</v>
       </c>
       <c r="E52" s="3">
@@ -2105,13 +2105,13 @@
       <c r="A53" s="17">
         <v>52</v>
       </c>
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="22">
+      <c r="D53" s="21">
         <v>1800</v>
       </c>
       <c r="E53" s="3">
@@ -2122,13 +2122,13 @@
       <c r="A54" s="17">
         <v>53</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="22">
+      <c r="D54" s="21">
         <v>1800</v>
       </c>
       <c r="E54" s="3">
@@ -2139,13 +2139,13 @@
       <c r="A55" s="17">
         <v>54</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="22">
+      <c r="D55" s="21">
         <v>1800</v>
       </c>
       <c r="E55" s="3">
@@ -2156,13 +2156,13 @@
       <c r="A56" s="17">
         <v>55</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="22">
+      <c r="D56" s="21">
         <v>1800</v>
       </c>
       <c r="E56" s="3">
@@ -2173,13 +2173,13 @@
       <c r="A57" s="17">
         <v>56</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="21">
         <v>1800</v>
       </c>
       <c r="E57" s="3">
@@ -2190,13 +2190,13 @@
       <c r="A58" s="17">
         <v>57</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="22">
+      <c r="D58" s="21">
         <v>1800</v>
       </c>
       <c r="E58" s="3">
@@ -2207,13 +2207,13 @@
       <c r="A59" s="17">
         <v>58</v>
       </c>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="22">
+      <c r="D59" s="21">
         <v>1800</v>
       </c>
       <c r="E59" s="3">
@@ -2224,13 +2224,13 @@
       <c r="A60" s="17">
         <v>59</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D60" s="22">
+      <c r="D60" s="21">
         <v>1800</v>
       </c>
       <c r="E60" s="3">
@@ -2241,13 +2241,13 @@
       <c r="A61" s="17">
         <v>60</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C61" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="22">
+      <c r="D61" s="21">
         <v>1800</v>
       </c>
       <c r="E61" s="3">
@@ -2258,13 +2258,13 @@
       <c r="A62" s="17">
         <v>61</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="22">
+      <c r="D62" s="21">
         <v>1800</v>
       </c>
       <c r="E62" s="3">
@@ -2275,13 +2275,13 @@
       <c r="A63" s="17">
         <v>62</v>
       </c>
-      <c r="B63" s="23" t="s">
+      <c r="B63" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="22">
+      <c r="D63" s="21">
         <v>1800</v>
       </c>
       <c r="E63" s="3">
@@ -2292,13 +2292,13 @@
       <c r="A64" s="17">
         <v>63</v>
       </c>
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="22">
+      <c r="D64" s="21">
         <v>1800</v>
       </c>
       <c r="E64" s="3">
@@ -2309,13 +2309,13 @@
       <c r="A65" s="17">
         <v>64</v>
       </c>
-      <c r="B65" s="23" t="s">
+      <c r="B65" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D65" s="22">
+      <c r="D65" s="21">
         <v>1800</v>
       </c>
       <c r="E65" s="3">
@@ -2326,13 +2326,13 @@
       <c r="A66" s="17">
         <v>65</v>
       </c>
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="22">
+      <c r="D66" s="21">
         <v>1800</v>
       </c>
       <c r="E66" s="3">
@@ -2343,13 +2343,13 @@
       <c r="A67" s="17">
         <v>66</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D67" s="22">
+      <c r="D67" s="21">
         <v>1800</v>
       </c>
       <c r="E67" s="3">
@@ -2360,13 +2360,13 @@
       <c r="A68" s="17">
         <v>67</v>
       </c>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="22">
+      <c r="D68" s="21">
         <v>1800</v>
       </c>
       <c r="E68" s="3">
@@ -2377,13 +2377,13 @@
       <c r="A69" s="17">
         <v>68</v>
       </c>
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="22">
+      <c r="D69" s="21">
         <v>1800</v>
       </c>
       <c r="E69" s="3">
@@ -2394,13 +2394,13 @@
       <c r="A70" s="17">
         <v>69</v>
       </c>
-      <c r="B70" s="23" t="s">
+      <c r="B70" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="22">
+      <c r="D70" s="21">
         <v>1800</v>
       </c>
       <c r="E70" s="3">
@@ -2411,13 +2411,13 @@
       <c r="A71" s="17">
         <v>70</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="22">
+      <c r="D71" s="21">
         <v>1800</v>
       </c>
       <c r="E71" s="3">
@@ -2428,13 +2428,13 @@
       <c r="A72" s="17">
         <v>71</v>
       </c>
-      <c r="B72" s="27" t="s">
+      <c r="B72" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="22">
+      <c r="D72" s="21">
         <v>1800</v>
       </c>
       <c r="E72" s="3">
@@ -2445,13 +2445,13 @@
       <c r="A73" s="17">
         <v>72</v>
       </c>
-      <c r="B73" s="27" t="s">
+      <c r="B73" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D73" s="22">
+      <c r="D73" s="21">
         <v>1800</v>
       </c>
       <c r="E73" s="3">
@@ -2462,13 +2462,13 @@
       <c r="A74" s="17">
         <v>73</v>
       </c>
-      <c r="B74" s="27">
+      <c r="B74" s="26">
         <v>100</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D74" s="22">
+      <c r="D74" s="21">
         <v>1800</v>
       </c>
       <c r="E74" s="3">
@@ -2479,13 +2479,13 @@
       <c r="A75" s="17">
         <v>74</v>
       </c>
-      <c r="B75" s="27" t="s">
+      <c r="B75" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="C75" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="22">
+      <c r="D75" s="21">
         <v>1800</v>
       </c>
       <c r="E75" s="3">
@@ -2496,13 +2496,13 @@
       <c r="A76" s="17">
         <v>75</v>
       </c>
-      <c r="B76" s="27" t="s">
+      <c r="B76" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="22">
+      <c r="D76" s="21">
         <v>1800</v>
       </c>
       <c r="E76" s="3">
@@ -2513,13 +2513,13 @@
       <c r="A77" s="17">
         <v>76</v>
       </c>
-      <c r="B77" s="27" t="s">
+      <c r="B77" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="22">
+      <c r="D77" s="21">
         <v>1800</v>
       </c>
       <c r="E77" s="3">
@@ -2530,13 +2530,13 @@
       <c r="A78" s="17">
         <v>77</v>
       </c>
-      <c r="B78" s="27" t="s">
+      <c r="B78" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C78" s="21" t="s">
+      <c r="C78" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D78" s="22">
+      <c r="D78" s="21">
         <v>1800</v>
       </c>
       <c r="E78" s="3">
@@ -2547,13 +2547,13 @@
       <c r="A79" s="17">
         <v>78</v>
       </c>
-      <c r="B79" s="27" t="s">
+      <c r="B79" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="C79" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="22">
+      <c r="D79" s="21">
         <v>1800</v>
       </c>
       <c r="E79" s="3">
@@ -2564,13 +2564,13 @@
       <c r="A80" s="17">
         <v>79</v>
       </c>
-      <c r="B80" s="27" t="s">
+      <c r="B80" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="21" t="s">
+      <c r="C80" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D80" s="22">
+      <c r="D80" s="21">
         <v>1800</v>
       </c>
       <c r="E80" s="3">
@@ -2581,13 +2581,13 @@
       <c r="A81" s="17">
         <v>80</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D81" s="22">
+      <c r="D81" s="21">
         <v>1800</v>
       </c>
       <c r="E81" s="3">
@@ -2598,13 +2598,13 @@
       <c r="A82" s="17">
         <v>81</v>
       </c>
-      <c r="B82" s="27" t="s">
+      <c r="B82" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D82" s="22">
+      <c r="D82" s="21">
         <v>1800</v>
       </c>
       <c r="E82" s="3">
@@ -2615,13 +2615,13 @@
       <c r="A83" s="17">
         <v>82</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C83" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="22">
+      <c r="D83" s="21">
         <v>1800</v>
       </c>
       <c r="E83" s="3">
@@ -2632,13 +2632,13 @@
       <c r="A84" s="17">
         <v>83</v>
       </c>
-      <c r="B84" s="27" t="s">
+      <c r="B84" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="22">
+      <c r="D84" s="21">
         <v>1800</v>
       </c>
       <c r="E84" s="3">
@@ -2649,13 +2649,13 @@
       <c r="A85" s="17">
         <v>84</v>
       </c>
-      <c r="B85" s="27" t="s">
+      <c r="B85" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="C85" s="21" t="s">
+      <c r="C85" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="22">
+      <c r="D85" s="21">
         <v>1800</v>
       </c>
       <c r="E85" s="3">
@@ -2666,13 +2666,13 @@
       <c r="A86" s="17">
         <v>85</v>
       </c>
-      <c r="B86" s="25" t="s">
+      <c r="B86" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C86" s="26" t="s">
+      <c r="C86" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D86" s="22">
+      <c r="D86" s="21">
         <v>1650</v>
       </c>
       <c r="E86" s="3">
@@ -2683,13 +2683,13 @@
       <c r="A87" s="17">
         <v>86</v>
       </c>
-      <c r="B87" s="25" t="s">
+      <c r="B87" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C87" s="26" t="s">
+      <c r="C87" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D87" s="22">
+      <c r="D87" s="21">
         <v>1650</v>
       </c>
       <c r="E87" s="3">
@@ -2700,13 +2700,13 @@
       <c r="A88" s="17">
         <v>87</v>
       </c>
-      <c r="B88" s="25" t="s">
+      <c r="B88" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C88" s="26" t="s">
+      <c r="C88" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D88" s="22">
+      <c r="D88" s="21">
         <v>1650</v>
       </c>
       <c r="E88" s="3">
@@ -2717,13 +2717,13 @@
       <c r="A89" s="17">
         <v>88</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="26" t="s">
+      <c r="C89" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D89" s="22">
+      <c r="D89" s="21">
         <v>1650</v>
       </c>
       <c r="E89" s="3">
@@ -2734,13 +2734,13 @@
       <c r="A90" s="17">
         <v>89</v>
       </c>
-      <c r="B90" s="25" t="s">
+      <c r="B90" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="26" t="s">
+      <c r="C90" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D90" s="22">
+      <c r="D90" s="21">
         <v>1650</v>
       </c>
       <c r="E90" s="3">
@@ -2751,13 +2751,13 @@
       <c r="A91" s="17">
         <v>90</v>
       </c>
-      <c r="B91" s="25" t="s">
+      <c r="B91" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D91" s="22">
+      <c r="D91" s="21">
         <v>1650</v>
       </c>
       <c r="E91" s="3">
@@ -2768,13 +2768,13 @@
       <c r="A92" s="17">
         <v>91</v>
       </c>
-      <c r="B92" s="25" t="s">
+      <c r="B92" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C92" s="26" t="s">
+      <c r="C92" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D92" s="22">
+      <c r="D92" s="21">
         <v>1650</v>
       </c>
       <c r="E92" s="3">
@@ -2785,13 +2785,13 @@
       <c r="A93" s="17">
         <v>92</v>
       </c>
-      <c r="B93" s="25" t="s">
+      <c r="B93" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D93" s="22">
+      <c r="D93" s="21">
         <v>1650</v>
       </c>
       <c r="E93" s="3">
@@ -2802,13 +2802,13 @@
       <c r="A94" s="17">
         <v>93</v>
       </c>
-      <c r="B94" s="25" t="s">
+      <c r="B94" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C94" s="26" t="s">
+      <c r="C94" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D94" s="22">
+      <c r="D94" s="21">
         <v>1650</v>
       </c>
       <c r="E94" s="3">
@@ -2819,13 +2819,13 @@
       <c r="A95" s="17">
         <v>94</v>
       </c>
-      <c r="B95" s="25" t="s">
+      <c r="B95" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C95" s="26" t="s">
+      <c r="C95" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D95" s="22">
+      <c r="D95" s="21">
         <v>1650</v>
       </c>
       <c r="E95" s="3">
@@ -2836,13 +2836,13 @@
       <c r="A96" s="17">
         <v>95</v>
       </c>
-      <c r="B96" s="25" t="s">
+      <c r="B96" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C96" s="26" t="s">
+      <c r="C96" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D96" s="22">
+      <c r="D96" s="21">
         <v>1650</v>
       </c>
       <c r="E96" s="3">
@@ -2853,13 +2853,13 @@
       <c r="A97" s="17">
         <v>96</v>
       </c>
-      <c r="B97" s="23" t="s">
+      <c r="B97" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C97" s="24" t="s">
+      <c r="C97" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D97" s="22">
+      <c r="D97" s="21">
         <v>1650</v>
       </c>
       <c r="E97" s="3">
@@ -2870,13 +2870,13 @@
       <c r="A98" s="17">
         <v>97</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="B98" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="24" t="s">
+      <c r="C98" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D98" s="22">
+      <c r="D98" s="21">
         <v>1650</v>
       </c>
       <c r="E98" s="3">
@@ -2887,13 +2887,13 @@
       <c r="A99" s="17">
         <v>98</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="24" t="s">
+      <c r="C99" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D99" s="22">
+      <c r="D99" s="21">
         <v>1650</v>
       </c>
       <c r="E99" s="3">
@@ -2904,13 +2904,13 @@
       <c r="A100" s="17">
         <v>99</v>
       </c>
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C100" s="24" t="s">
+      <c r="C100" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D100" s="22">
+      <c r="D100" s="21">
         <v>1650</v>
       </c>
       <c r="E100" s="3">
@@ -2921,13 +2921,13 @@
       <c r="A101" s="17">
         <v>100</v>
       </c>
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C101" s="24" t="s">
+      <c r="C101" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D101" s="22">
+      <c r="D101" s="21">
         <v>1650</v>
       </c>
       <c r="E101" s="3">
@@ -2938,13 +2938,13 @@
       <c r="A102" s="17">
         <v>101</v>
       </c>
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C102" s="24" t="s">
+      <c r="C102" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D102" s="22">
+      <c r="D102" s="21">
         <v>1650</v>
       </c>
       <c r="E102" s="3">
@@ -2955,13 +2955,13 @@
       <c r="A103" s="17">
         <v>102</v>
       </c>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="C103" s="24" t="s">
+      <c r="C103" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D103" s="22">
+      <c r="D103" s="21">
         <v>1650</v>
       </c>
       <c r="E103" s="3">
@@ -2972,13 +2972,13 @@
       <c r="A104" s="17">
         <v>103</v>
       </c>
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="C104" s="24" t="s">
+      <c r="C104" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D104" s="22">
+      <c r="D104" s="21">
         <v>1650</v>
       </c>
       <c r="E104" s="3">
@@ -2989,13 +2989,13 @@
       <c r="A105" s="17">
         <v>104</v>
       </c>
-      <c r="B105" s="23" t="s">
+      <c r="B105" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C105" s="24" t="s">
+      <c r="C105" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="22">
+      <c r="D105" s="21">
         <v>1650</v>
       </c>
       <c r="E105" s="3">
@@ -3006,13 +3006,13 @@
       <c r="A106" s="17">
         <v>105</v>
       </c>
-      <c r="B106" s="27" t="s">
+      <c r="B106" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C106" s="21" t="s">
+      <c r="C106" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D106" s="22">
+      <c r="D106" s="21">
         <v>1650</v>
       </c>
       <c r="E106" s="3">
@@ -3023,13 +3023,13 @@
       <c r="A107" s="17">
         <v>106</v>
       </c>
-      <c r="B107" s="27" t="s">
+      <c r="B107" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C107" s="21" t="s">
+      <c r="C107" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D107" s="22">
+      <c r="D107" s="21">
         <v>1650</v>
       </c>
       <c r="E107" s="3">
@@ -3040,13 +3040,13 @@
       <c r="A108" s="17">
         <v>107</v>
       </c>
-      <c r="B108" s="27" t="s">
+      <c r="B108" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C108" s="21" t="s">
+      <c r="C108" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D108" s="22">
+      <c r="D108" s="21">
         <v>1650</v>
       </c>
       <c r="E108" s="3">
@@ -3057,13 +3057,13 @@
       <c r="A109" s="17">
         <v>108</v>
       </c>
-      <c r="B109" s="27" t="s">
+      <c r="B109" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="C109" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D109" s="22">
+      <c r="D109" s="21">
         <v>1650</v>
       </c>
       <c r="E109" s="3">
@@ -3074,13 +3074,13 @@
       <c r="A110" s="17">
         <v>109</v>
       </c>
-      <c r="B110" s="27" t="s">
+      <c r="B110" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="21" t="s">
+      <c r="C110" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D110" s="22">
+      <c r="D110" s="21">
         <v>1650</v>
       </c>
       <c r="E110" s="3">
@@ -3091,13 +3091,13 @@
       <c r="A111" s="17">
         <v>110</v>
       </c>
-      <c r="B111" s="27" t="s">
+      <c r="B111" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C111" s="21" t="s">
+      <c r="C111" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D111" s="22">
+      <c r="D111" s="21">
         <v>1650</v>
       </c>
       <c r="E111" s="3">
@@ -3108,13 +3108,13 @@
       <c r="A112" s="17">
         <v>111</v>
       </c>
-      <c r="B112" s="25" t="s">
+      <c r="B112" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C112" s="26" t="s">
+      <c r="C112" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D112" s="22">
+      <c r="D112" s="21">
         <v>1650</v>
       </c>
       <c r="E112" s="3">
@@ -3125,13 +3125,13 @@
       <c r="A113" s="17">
         <v>112</v>
       </c>
-      <c r="B113" s="25" t="s">
+      <c r="B113" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C113" s="26" t="s">
+      <c r="C113" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D113" s="22">
+      <c r="D113" s="21">
         <v>1650</v>
       </c>
       <c r="E113" s="3">
@@ -3142,13 +3142,13 @@
       <c r="A114" s="17">
         <v>113</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="B114" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C114" s="26" t="s">
+      <c r="C114" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D114" s="22">
+      <c r="D114" s="21">
         <v>1650</v>
       </c>
       <c r="E114" s="3">
@@ -3159,13 +3159,13 @@
       <c r="A115" s="17">
         <v>114</v>
       </c>
-      <c r="B115" s="25" t="s">
+      <c r="B115" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C115" s="26" t="s">
+      <c r="C115" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D115" s="22">
+      <c r="D115" s="21">
         <v>1650</v>
       </c>
       <c r="E115" s="3">
@@ -3176,13 +3176,13 @@
       <c r="A116" s="17">
         <v>115</v>
       </c>
-      <c r="B116" s="25" t="s">
+      <c r="B116" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="C116" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D116" s="22">
+      <c r="D116" s="21">
         <v>1650</v>
       </c>
       <c r="E116" s="3">
@@ -3193,13 +3193,13 @@
       <c r="A117" s="17">
         <v>116</v>
       </c>
-      <c r="B117" s="28" t="s">
+      <c r="B117" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C117" s="29" t="s">
+      <c r="C117" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D117" s="22">
+      <c r="D117" s="21">
         <v>1650</v>
       </c>
       <c r="E117" s="3">
@@ -3210,13 +3210,13 @@
       <c r="A118" s="17">
         <v>117</v>
       </c>
-      <c r="B118" s="28" t="s">
+      <c r="B118" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C118" s="29" t="s">
+      <c r="C118" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D118" s="22">
+      <c r="D118" s="21">
         <v>1650</v>
       </c>
       <c r="E118" s="3">
@@ -3227,13 +3227,13 @@
       <c r="A119" s="17">
         <v>118</v>
       </c>
-      <c r="B119" s="28" t="s">
+      <c r="B119" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C119" s="29" t="s">
+      <c r="C119" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D119" s="22">
+      <c r="D119" s="21">
         <v>1650</v>
       </c>
       <c r="E119" s="3">
@@ -3244,13 +3244,13 @@
       <c r="A120" s="17">
         <v>119</v>
       </c>
-      <c r="B120" s="28" t="s">
+      <c r="B120" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="C120" s="29" t="s">
+      <c r="C120" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D120" s="22">
+      <c r="D120" s="21">
         <v>1650</v>
       </c>
       <c r="E120" s="3">
@@ -3261,13 +3261,13 @@
       <c r="A121" s="17">
         <v>120</v>
       </c>
-      <c r="B121" s="28" t="s">
+      <c r="B121" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="C121" s="29" t="s">
+      <c r="C121" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D121" s="22">
+      <c r="D121" s="21">
         <v>1650</v>
       </c>
       <c r="E121" s="3">
@@ -3278,13 +3278,13 @@
       <c r="A122" s="17">
         <v>121</v>
       </c>
-      <c r="B122" s="28" t="s">
+      <c r="B122" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C122" s="29" t="s">
+      <c r="C122" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D122" s="22">
+      <c r="D122" s="21">
         <v>1650</v>
       </c>
       <c r="E122" s="3">
@@ -3295,13 +3295,13 @@
       <c r="A123" s="17">
         <v>122</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="B123" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C123" s="29" t="s">
+      <c r="C123" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D123" s="22">
+      <c r="D123" s="21">
         <v>1650</v>
       </c>
       <c r="E123" s="3">
@@ -3312,13 +3312,13 @@
       <c r="A124" s="17">
         <v>123</v>
       </c>
-      <c r="B124" s="28" t="s">
+      <c r="B124" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C124" s="29" t="s">
+      <c r="C124" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="D124" s="22">
+      <c r="D124" s="21">
         <v>1650</v>
       </c>
       <c r="E124" s="3">
@@ -3329,13 +3329,13 @@
       <c r="A125" s="17">
         <v>124</v>
       </c>
-      <c r="B125" s="27" t="s">
+      <c r="B125" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="21" t="s">
+      <c r="C125" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D125" s="22">
+      <c r="D125" s="21">
         <v>1650</v>
       </c>
       <c r="E125" s="3">
@@ -3346,13 +3346,13 @@
       <c r="A126" s="17">
         <v>125</v>
       </c>
-      <c r="B126" s="27" t="s">
+      <c r="B126" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C126" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D126" s="22">
+      <c r="D126" s="21">
         <v>1650</v>
       </c>
       <c r="E126" s="3">
@@ -3363,13 +3363,13 @@
       <c r="A127" s="17">
         <v>126</v>
       </c>
-      <c r="B127" s="27" t="s">
+      <c r="B127" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="21" t="s">
+      <c r="C127" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D127" s="22">
+      <c r="D127" s="21">
         <v>1650</v>
       </c>
       <c r="E127" s="3">
@@ -3380,13 +3380,13 @@
       <c r="A128" s="17">
         <v>127</v>
       </c>
-      <c r="B128" s="27" t="s">
+      <c r="B128" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C128" s="21" t="s">
+      <c r="C128" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D128" s="22">
+      <c r="D128" s="21">
         <v>1650</v>
       </c>
       <c r="E128" s="3">
@@ -3397,13 +3397,13 @@
       <c r="A129" s="17">
         <v>128</v>
       </c>
-      <c r="B129" s="27" t="s">
+      <c r="B129" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C129" s="21" t="s">
+      <c r="C129" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D129" s="22">
+      <c r="D129" s="21">
         <v>1650</v>
       </c>
       <c r="E129" s="3">
@@ -3414,13 +3414,13 @@
       <c r="A130" s="17">
         <v>129</v>
       </c>
-      <c r="B130" s="27" t="s">
+      <c r="B130" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="21" t="s">
+      <c r="C130" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D130" s="22">
+      <c r="D130" s="21">
         <v>1650</v>
       </c>
       <c r="E130" s="3">
@@ -3431,13 +3431,13 @@
       <c r="A131" s="17">
         <v>130</v>
       </c>
-      <c r="B131" s="27" t="s">
+      <c r="B131" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C131" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D131" s="22">
+      <c r="D131" s="21">
         <v>1650</v>
       </c>
       <c r="E131" s="3">
@@ -3448,13 +3448,13 @@
       <c r="A132" s="17">
         <v>131</v>
       </c>
-      <c r="B132" s="27" t="s">
+      <c r="B132" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C132" s="21" t="s">
+      <c r="C132" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D132" s="22">
+      <c r="D132" s="21">
         <v>1650</v>
       </c>
       <c r="E132" s="3">
@@ -3465,13 +3465,13 @@
       <c r="A133" s="17">
         <v>132</v>
       </c>
-      <c r="B133" s="27" t="s">
+      <c r="B133" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C133" s="21" t="s">
+      <c r="C133" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D133" s="22">
+      <c r="D133" s="21">
         <v>1650</v>
       </c>
       <c r="E133" s="3">
@@ -3482,13 +3482,13 @@
       <c r="A134" s="17">
         <v>133</v>
       </c>
-      <c r="B134" s="27" t="s">
+      <c r="B134" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="C134" s="21" t="s">
+      <c r="C134" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D134" s="22">
+      <c r="D134" s="21">
         <v>1650</v>
       </c>
       <c r="E134" s="3">
@@ -3499,13 +3499,13 @@
       <c r="A135" s="17">
         <v>134</v>
       </c>
-      <c r="B135" s="27" t="s">
+      <c r="B135" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C135" s="21" t="s">
+      <c r="C135" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D135" s="22">
+      <c r="D135" s="21">
         <v>1650</v>
       </c>
       <c r="E135" s="3">
@@ -3516,13 +3516,13 @@
       <c r="A136" s="17">
         <v>135</v>
       </c>
-      <c r="B136" s="27" t="s">
+      <c r="B136" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C136" s="21" t="s">
+      <c r="C136" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D136" s="22">
+      <c r="D136" s="21">
         <v>1650</v>
       </c>
       <c r="E136" s="3">
@@ -3533,13 +3533,13 @@
       <c r="A137" s="17">
         <v>136</v>
       </c>
-      <c r="B137" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C137" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D137" s="22">
+      <c r="B137" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C137" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D137" s="21">
         <v>1650</v>
       </c>
       <c r="E137" s="3">
@@ -3550,13 +3550,13 @@
       <c r="A138" s="17">
         <v>137</v>
       </c>
-      <c r="B138" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C138" s="26" t="s">
+      <c r="B138" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C138" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D138" s="22">
+      <c r="D138" s="21">
         <v>1650</v>
       </c>
       <c r="E138" s="3">
@@ -3567,13 +3567,13 @@
       <c r="A139" s="17">
         <v>138</v>
       </c>
-      <c r="B139" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="C139" s="26" t="s">
+      <c r="B139" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C139" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D139" s="22">
+      <c r="D139" s="21">
         <v>1650</v>
       </c>
       <c r="E139" s="3">
@@ -3584,13 +3584,13 @@
       <c r="A140" s="17">
         <v>139</v>
       </c>
-      <c r="B140" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C140" s="26" t="s">
+      <c r="B140" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C140" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D140" s="22">
+      <c r="D140" s="21">
         <v>1650</v>
       </c>
       <c r="E140" s="3">
@@ -3601,13 +3601,13 @@
       <c r="A141" s="17">
         <v>140</v>
       </c>
-      <c r="B141" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C141" s="26" t="s">
+      <c r="B141" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C141" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D141" s="22">
+      <c r="D141" s="21">
         <v>1650</v>
       </c>
       <c r="E141" s="3">
@@ -3618,13 +3618,13 @@
       <c r="A142" s="17">
         <v>141</v>
       </c>
-      <c r="B142" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C142" s="26" t="s">
+      <c r="B142" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C142" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D142" s="22">
+      <c r="D142" s="21">
         <v>1650</v>
       </c>
       <c r="E142" s="3">
@@ -3635,13 +3635,13 @@
       <c r="A143" s="17">
         <v>142</v>
       </c>
-      <c r="B143" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C143" s="26" t="s">
+      <c r="B143" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C143" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D143" s="22">
+      <c r="D143" s="21">
         <v>1650</v>
       </c>
       <c r="E143" s="3">
@@ -3652,13 +3652,13 @@
       <c r="A144" s="17">
         <v>143</v>
       </c>
-      <c r="B144" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C144" s="26" t="s">
+      <c r="B144" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C144" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D144" s="22">
+      <c r="D144" s="21">
         <v>1650</v>
       </c>
       <c r="E144" s="3">
@@ -3669,13 +3669,13 @@
       <c r="A145" s="17">
         <v>144</v>
       </c>
-      <c r="B145" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C145" s="26" t="s">
+      <c r="B145" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C145" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D145" s="22">
+      <c r="D145" s="21">
         <v>1650</v>
       </c>
       <c r="E145" s="3">
@@ -3686,13 +3686,13 @@
       <c r="A146" s="17">
         <v>145</v>
       </c>
-      <c r="B146" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C146" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D146" s="22">
+      <c r="B146" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C146" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D146" s="21">
         <v>1650</v>
       </c>
       <c r="E146" s="3">
@@ -3703,13 +3703,13 @@
       <c r="A147" s="17">
         <v>146</v>
       </c>
-      <c r="B147" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C147" s="24" t="s">
+      <c r="B147" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C147" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D147" s="22">
+      <c r="D147" s="21">
         <v>1650</v>
       </c>
       <c r="E147" s="3">
@@ -3720,13 +3720,13 @@
       <c r="A148" s="17">
         <v>147</v>
       </c>
-      <c r="B148" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C148" s="24" t="s">
+      <c r="B148" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C148" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D148" s="22">
+      <c r="D148" s="21">
         <v>1650</v>
       </c>
       <c r="E148" s="3">
@@ -3737,13 +3737,13 @@
       <c r="A149" s="17">
         <v>148</v>
       </c>
-      <c r="B149" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C149" s="24" t="s">
+      <c r="B149" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C149" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D149" s="22">
+      <c r="D149" s="21">
         <v>1650</v>
       </c>
       <c r="E149" s="3">
@@ -3754,13 +3754,13 @@
       <c r="A150" s="17">
         <v>149</v>
       </c>
-      <c r="B150" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C150" s="24" t="s">
+      <c r="B150" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C150" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D150" s="22">
+      <c r="D150" s="21">
         <v>1650</v>
       </c>
       <c r="E150" s="3">
@@ -3771,13 +3771,13 @@
       <c r="A151" s="17">
         <v>150</v>
       </c>
-      <c r="B151" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C151" s="24" t="s">
+      <c r="B151" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C151" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D151" s="22">
+      <c r="D151" s="21">
         <v>1650</v>
       </c>
       <c r="E151" s="3">
@@ -3788,13 +3788,13 @@
       <c r="A152" s="17">
         <v>151</v>
       </c>
-      <c r="B152" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C152" s="24" t="s">
+      <c r="B152" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C152" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D152" s="22">
+      <c r="D152" s="21">
         <v>1650</v>
       </c>
       <c r="E152" s="3">
@@ -3805,13 +3805,13 @@
       <c r="A153" s="17">
         <v>152</v>
       </c>
-      <c r="B153" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C153" s="24" t="s">
+      <c r="B153" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C153" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D153" s="22">
+      <c r="D153" s="21">
         <v>1650</v>
       </c>
       <c r="E153" s="3">
@@ -3822,13 +3822,13 @@
       <c r="A154" s="17">
         <v>153</v>
       </c>
-      <c r="B154" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C154" s="24" t="s">
+      <c r="B154" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C154" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D154" s="22">
+      <c r="D154" s="21">
         <v>1650</v>
       </c>
       <c r="E154" s="3">
@@ -3839,13 +3839,13 @@
       <c r="A155" s="17">
         <v>154</v>
       </c>
-      <c r="B155" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C155" s="24" t="s">
+      <c r="B155" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C155" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D155" s="22">
+      <c r="D155" s="21">
         <v>1650</v>
       </c>
       <c r="E155" s="3">
@@ -3856,13 +3856,13 @@
       <c r="A156" s="17">
         <v>155</v>
       </c>
-      <c r="B156" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C156" s="24" t="s">
+      <c r="B156" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C156" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D156" s="22">
+      <c r="D156" s="21">
         <v>1650</v>
       </c>
       <c r="E156" s="3">
@@ -3873,13 +3873,13 @@
       <c r="A157" s="17">
         <v>156</v>
       </c>
-      <c r="B157" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="C157" s="24" t="s">
+      <c r="B157" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C157" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D157" s="22">
+      <c r="D157" s="21">
         <v>1650</v>
       </c>
       <c r="E157" s="3">
@@ -3890,13 +3890,13 @@
       <c r="A158" s="17">
         <v>157</v>
       </c>
-      <c r="B158" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C158" s="24" t="s">
+      <c r="B158" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C158" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D158" s="22">
+      <c r="D158" s="21">
         <v>1650</v>
       </c>
       <c r="E158" s="3">
@@ -3907,13 +3907,13 @@
       <c r="A159" s="17">
         <v>158</v>
       </c>
-      <c r="B159" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C159" s="24" t="s">
+      <c r="B159" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C159" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D159" s="22">
+      <c r="D159" s="21">
         <v>1650</v>
       </c>
       <c r="E159" s="3">
@@ -3924,13 +3924,13 @@
       <c r="A160" s="17">
         <v>159</v>
       </c>
-      <c r="B160" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="C160" s="24" t="s">
+      <c r="B160" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C160" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D160" s="22">
+      <c r="D160" s="21">
         <v>1650</v>
       </c>
       <c r="E160" s="3">
@@ -3941,13 +3941,13 @@
       <c r="A161" s="17">
         <v>160</v>
       </c>
-      <c r="B161" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C161" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D161" s="22">
+      <c r="B161" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C161" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D161" s="21">
         <v>1650</v>
       </c>
       <c r="E161" s="3">
@@ -3958,13 +3958,13 @@
       <c r="A162" s="17">
         <v>161</v>
       </c>
-      <c r="B162" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C162" s="21" t="s">
+      <c r="B162" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C162" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D162" s="22">
+      <c r="D162" s="21">
         <v>1650</v>
       </c>
       <c r="E162" s="3">
@@ -3975,13 +3975,13 @@
       <c r="A163" s="17">
         <v>162</v>
       </c>
-      <c r="B163" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C163" s="21" t="s">
+      <c r="B163" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C163" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D163" s="22">
+      <c r="D163" s="21">
         <v>1650</v>
       </c>
       <c r="E163" s="3">
@@ -3992,13 +3992,13 @@
       <c r="A164" s="17">
         <v>163</v>
       </c>
-      <c r="B164" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C164" s="21" t="s">
+      <c r="B164" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C164" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D164" s="22">
+      <c r="D164" s="21">
         <v>1650</v>
       </c>
       <c r="E164" s="3">
@@ -4009,13 +4009,13 @@
       <c r="A165" s="17">
         <v>164</v>
       </c>
-      <c r="B165" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="C165" s="21" t="s">
+      <c r="B165" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C165" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D165" s="22">
+      <c r="D165" s="21">
         <v>1650</v>
       </c>
       <c r="E165" s="3">
@@ -4026,13 +4026,13 @@
       <c r="A166" s="17">
         <v>165</v>
       </c>
-      <c r="B166" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="C166" s="21" t="s">
+      <c r="B166" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C166" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D166" s="22">
+      <c r="D166" s="21">
         <v>1650</v>
       </c>
       <c r="E166" s="3">
@@ -4043,13 +4043,13 @@
       <c r="A167" s="17">
         <v>166</v>
       </c>
-      <c r="B167" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C167" s="21" t="s">
+      <c r="B167" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C167" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D167" s="22">
+      <c r="D167" s="21">
         <v>1650</v>
       </c>
       <c r="E167" s="3">
@@ -4060,13 +4060,13 @@
       <c r="A168" s="17">
         <v>167</v>
       </c>
-      <c r="B168" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="C168" s="21" t="s">
+      <c r="B168" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C168" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D168" s="22">
+      <c r="D168" s="21">
         <v>1650</v>
       </c>
       <c r="E168" s="3">
@@ -4077,13 +4077,13 @@
       <c r="A169" s="17">
         <v>168</v>
       </c>
-      <c r="B169" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="C169" s="21" t="s">
+      <c r="B169" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C169" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D169" s="22">
+      <c r="D169" s="21">
         <v>1650</v>
       </c>
       <c r="E169" s="3">
@@ -4094,13 +4094,13 @@
       <c r="A170" s="17">
         <v>169</v>
       </c>
-      <c r="B170" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="C170" s="21" t="s">
+      <c r="B170" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C170" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D170" s="22">
+      <c r="D170" s="21">
         <v>1650</v>
       </c>
       <c r="E170" s="3">
@@ -4111,13 +4111,13 @@
       <c r="A171" s="17">
         <v>170</v>
       </c>
-      <c r="B171" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C171" s="21" t="s">
+      <c r="B171" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C171" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D171" s="22">
+      <c r="D171" s="21">
         <v>1650</v>
       </c>
       <c r="E171" s="3">
@@ -4128,13 +4128,13 @@
       <c r="A172" s="17">
         <v>171</v>
       </c>
-      <c r="B172" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C172" s="21" t="s">
+      <c r="B172" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C172" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D172" s="22">
+      <c r="D172" s="21">
         <v>1650</v>
       </c>
       <c r="E172" s="3">
@@ -4145,13 +4145,13 @@
       <c r="A173" s="17">
         <v>172</v>
       </c>
-      <c r="B173" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C173" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D173" s="22">
+      <c r="B173" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C173" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D173" s="21">
         <v>1650</v>
       </c>
       <c r="E173" s="3">
@@ -4162,13 +4162,13 @@
       <c r="A174" s="17">
         <v>173</v>
       </c>
-      <c r="B174" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="C174" s="26" t="s">
+      <c r="B174" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C174" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D174" s="22">
+      <c r="D174" s="21">
         <v>1650</v>
       </c>
       <c r="E174" s="3">
@@ -4179,13 +4179,13 @@
       <c r="A175" s="17">
         <v>174</v>
       </c>
-      <c r="B175" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C175" s="26" t="s">
+      <c r="B175" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C175" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D175" s="22">
+      <c r="D175" s="21">
         <v>1650</v>
       </c>
       <c r="E175" s="3">
@@ -4196,13 +4196,13 @@
       <c r="A176" s="17">
         <v>175</v>
       </c>
-      <c r="B176" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C176" s="26" t="s">
+      <c r="B176" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C176" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D176" s="22">
+      <c r="D176" s="21">
         <v>1650</v>
       </c>
       <c r="E176" s="3">
@@ -4213,13 +4213,13 @@
       <c r="A177" s="17">
         <v>176</v>
       </c>
-      <c r="B177" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C177" s="26" t="s">
+      <c r="B177" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C177" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D177" s="22">
+      <c r="D177" s="21">
         <v>1650</v>
       </c>
       <c r="E177" s="3">
@@ -4230,13 +4230,13 @@
       <c r="A178" s="17">
         <v>177</v>
       </c>
-      <c r="B178" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C178" s="26" t="s">
+      <c r="B178" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C178" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D178" s="22">
+      <c r="D178" s="21">
         <v>1650</v>
       </c>
       <c r="E178" s="3">
@@ -4247,13 +4247,13 @@
       <c r="A179" s="17">
         <v>178</v>
       </c>
-      <c r="B179" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C179" s="26" t="s">
+      <c r="B179" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C179" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D179" s="22">
+      <c r="D179" s="21">
         <v>1650</v>
       </c>
       <c r="E179" s="3">
@@ -4264,13 +4264,13 @@
       <c r="A180" s="17">
         <v>179</v>
       </c>
-      <c r="B180" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="C180" s="26" t="s">
+      <c r="B180" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C180" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D180" s="22">
+      <c r="D180" s="21">
         <v>1650</v>
       </c>
       <c r="E180" s="3">
@@ -4281,13 +4281,13 @@
       <c r="A181" s="17">
         <v>180</v>
       </c>
-      <c r="B181" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="C181" s="26" t="s">
+      <c r="B181" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C181" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D181" s="22">
+      <c r="D181" s="21">
         <v>1650</v>
       </c>
       <c r="E181" s="3">
@@ -4298,39 +4298,52 @@
       <c r="A182" s="17">
         <v>181</v>
       </c>
-      <c r="B182" s="25" t="s">
+      <c r="B182" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C182" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D182" s="21">
+        <v>1650</v>
+      </c>
+      <c r="E182" s="3">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="17">
+        <v>182</v>
+      </c>
+      <c r="B183" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="C182" s="26" t="s">
+      <c r="C183" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D182" s="22">
-        <v>1650</v>
-      </c>
-      <c r="E182" s="3">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A183" s="18">
-        <v>182</v>
-      </c>
-      <c r="B183" s="14" t="s">
+      <c r="D183" s="21">
+        <v>1650</v>
+      </c>
+      <c r="E183" s="3">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A184" s="18">
+        <v>183</v>
+      </c>
+      <c r="B184" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="C183" s="15" t="s">
+      <c r="C184" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D183" s="2">
-        <v>1650</v>
-      </c>
-      <c r="E183" s="4">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A184"/>
-      <c r="B184" s="19"/>
+      <c r="D184" s="2">
+        <v>1650</v>
+      </c>
+      <c r="E184" s="4">
+        <v>1650</v>
+      </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185"/>

</xml_diff>

<commit_message>
Making functions to predict past matches with past knowledge
</commit_message>
<xml_diff>
--- a/TIMES.xlsx
+++ b/TIMES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bruno Almeida\Documentos\Faculdade\Games_Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051AC38C-A076-411A-8E78-148E86B98BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344EDD54-672D-4F5A-BD9C-4D7852631530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,7 +733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -749,55 +749,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -840,63 +791,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -915,6 +821,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G181" sqref="G181"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,77 +1118,77 @@
     <col min="9" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="16">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <v>1850</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>1850</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="9">
         <v>1850</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="9">
         <v>1850</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="9">
         <v>1850</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1289,16 +1196,16 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="9">
         <v>1850</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1306,16 +1213,16 @@
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="9">
         <v>1850</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1323,16 +1230,16 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="9">
         <v>1850</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1340,16 +1247,16 @@
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="9">
         <v>1850</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1357,16 +1264,16 @@
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="9">
         <v>1850</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1374,16 +1281,16 @@
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="9">
         <v>1850</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1391,16 +1298,16 @@
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="9">
         <v>1850</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1408,16 +1315,16 @@
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="9">
         <v>1850</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1425,16 +1332,16 @@
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="9">
         <v>1850</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1442,16 +1349,16 @@
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="9">
         <v>1850</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1459,16 +1366,16 @@
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="9">
         <v>1850</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1476,16 +1383,16 @@
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="9">
         <v>1850</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1493,16 +1400,16 @@
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="9">
         <v>1850</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1510,16 +1417,16 @@
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="9">
         <v>1850</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1527,16 +1434,16 @@
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="9">
         <v>1850</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1544,16 +1451,16 @@
       <c r="A20" s="17">
         <v>19</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="9">
         <v>1850</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="9">
         <v>1850</v>
       </c>
     </row>
@@ -1561,16 +1468,16 @@
       <c r="A21" s="17">
         <v>20</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D21" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E21" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1578,16 +1485,16 @@
       <c r="A22" s="17">
         <v>21</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D22" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E22" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1595,16 +1502,16 @@
       <c r="A23" s="17">
         <v>22</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E23" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1612,16 +1519,16 @@
       <c r="A24" s="17">
         <v>23</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="D24" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E24" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1629,16 +1536,16 @@
       <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="D25" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E25" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1646,16 +1553,16 @@
       <c r="A26" s="17">
         <v>25</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="D26" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E26" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1663,16 +1570,16 @@
       <c r="A27" s="17">
         <v>26</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="D27" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E27" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1680,16 +1587,16 @@
       <c r="A28" s="17">
         <v>27</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="D28" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E28" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1697,16 +1604,16 @@
       <c r="A29" s="17">
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="D29" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E29" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1714,16 +1621,16 @@
       <c r="A30" s="17">
         <v>29</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="D30" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E30" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1731,16 +1638,16 @@
       <c r="A31" s="17">
         <v>30</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="D31" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E31" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1748,16 +1655,16 @@
       <c r="A32" s="17">
         <v>31</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="D32" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E32" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1765,16 +1672,16 @@
       <c r="A33" s="17">
         <v>32</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="D33" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E33" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1782,16 +1689,16 @@
       <c r="A34" s="17">
         <v>33</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E34" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1799,16 +1706,16 @@
       <c r="A35" s="17">
         <v>34</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="D35" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E35" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1816,16 +1723,16 @@
       <c r="A36" s="17">
         <v>35</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E36" s="3">
+      <c r="D36" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E36" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1833,16 +1740,16 @@
       <c r="A37" s="17">
         <v>36</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D37" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E37" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1850,16 +1757,16 @@
       <c r="A38" s="17">
         <v>37</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="D38" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E38" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1867,16 +1774,16 @@
       <c r="A39" s="17">
         <v>38</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E39" s="3">
+      <c r="D39" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E39" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -1884,16 +1791,16 @@
       <c r="A40" s="17">
         <v>39</v>
       </c>
-      <c r="B40" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="25" t="s">
+      <c r="B40" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="9">
         <v>1750</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1901,16 +1808,16 @@
       <c r="A41" s="17">
         <v>40</v>
       </c>
-      <c r="B41" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="25" t="s">
+      <c r="B41" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="21">
+      <c r="D41" s="9">
         <v>1750</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1918,16 +1825,16 @@
       <c r="A42" s="17">
         <v>41</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="9">
         <v>1750</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1935,16 +1842,16 @@
       <c r="A43" s="17">
         <v>42</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="9">
         <v>1750</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1952,16 +1859,16 @@
       <c r="A44" s="17">
         <v>43</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="9">
         <v>1750</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1969,16 +1876,16 @@
       <c r="A45" s="17">
         <v>44</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="9">
         <v>1750</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -1986,16 +1893,16 @@
       <c r="A46" s="17">
         <v>45</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="9">
         <v>1750</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2003,16 +1910,16 @@
       <c r="A47" s="17">
         <v>46</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="9">
         <v>1750</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2020,16 +1927,16 @@
       <c r="A48" s="17">
         <v>47</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="9">
         <v>1750</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2037,16 +1944,16 @@
       <c r="A49" s="17">
         <v>48</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="9">
         <v>1750</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2054,16 +1961,16 @@
       <c r="A50" s="17">
         <v>49</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="9">
         <v>1750</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2071,16 +1978,16 @@
       <c r="A51" s="17">
         <v>50</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="21">
+      <c r="D51" s="9">
         <v>1750</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="9">
         <v>1750</v>
       </c>
     </row>
@@ -2088,33 +1995,33 @@
       <c r="A52" s="17">
         <v>51</v>
       </c>
-      <c r="B52" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D52" s="21">
-        <v>1750</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1750</v>
+      <c r="B52" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E52" s="9">
+        <v>1800</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="17">
         <v>52</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E53" s="3">
+      <c r="D53" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E53" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2122,16 +2029,16 @@
       <c r="A54" s="17">
         <v>53</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E54" s="3">
+      <c r="D54" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E54" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2139,16 +2046,16 @@
       <c r="A55" s="17">
         <v>54</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="C55" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E55" s="3">
+      <c r="D55" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E55" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2156,16 +2063,16 @@
       <c r="A56" s="17">
         <v>55</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E56" s="3">
+      <c r="D56" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E56" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2173,16 +2080,16 @@
       <c r="A57" s="17">
         <v>56</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E57" s="3">
+      <c r="D57" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E57" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2190,16 +2097,16 @@
       <c r="A58" s="17">
         <v>57</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E58" s="3">
+      <c r="D58" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E58" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2207,16 +2114,16 @@
       <c r="A59" s="17">
         <v>58</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E59" s="3">
+      <c r="D59" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E59" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2224,16 +2131,16 @@
       <c r="A60" s="17">
         <v>59</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="23" t="s">
+      <c r="C60" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D60" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E60" s="3">
+      <c r="D60" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E60" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2241,16 +2148,16 @@
       <c r="A61" s="17">
         <v>60</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E61" s="3">
+      <c r="D61" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E61" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2258,16 +2165,16 @@
       <c r="A62" s="17">
         <v>61</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C62" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E62" s="3">
+      <c r="D62" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E62" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2275,16 +2182,16 @@
       <c r="A63" s="17">
         <v>62</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E63" s="3">
+      <c r="D63" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E63" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2292,16 +2199,16 @@
       <c r="A64" s="17">
         <v>63</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E64" s="3">
+      <c r="D64" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E64" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2309,16 +2216,16 @@
       <c r="A65" s="17">
         <v>64</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D65" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E65" s="3">
+      <c r="D65" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E65" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2326,16 +2233,16 @@
       <c r="A66" s="17">
         <v>65</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="23" t="s">
+      <c r="C66" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E66" s="3">
+      <c r="D66" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E66" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2343,16 +2250,16 @@
       <c r="A67" s="17">
         <v>66</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D67" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E67" s="3">
+      <c r="D67" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E67" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2360,16 +2267,16 @@
       <c r="A68" s="17">
         <v>67</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C68" s="23" t="s">
+      <c r="C68" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E68" s="3">
+      <c r="D68" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E68" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2377,16 +2284,16 @@
       <c r="A69" s="17">
         <v>68</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="23" t="s">
+      <c r="C69" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E69" s="3">
+      <c r="D69" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E69" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2394,16 +2301,16 @@
       <c r="A70" s="17">
         <v>69</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="23" t="s">
+      <c r="C70" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E70" s="3">
+      <c r="D70" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E70" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2411,16 +2318,16 @@
       <c r="A71" s="17">
         <v>70</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="23" t="s">
+      <c r="C71" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E71" s="3">
+      <c r="D71" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E71" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2428,16 +2335,16 @@
       <c r="A72" s="17">
         <v>71</v>
       </c>
-      <c r="B72" s="26" t="s">
+      <c r="B72" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E72" s="3">
+      <c r="D72" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E72" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2445,16 +2352,16 @@
       <c r="A73" s="17">
         <v>72</v>
       </c>
-      <c r="B73" s="26" t="s">
+      <c r="B73" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D73" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E73" s="3">
+      <c r="D73" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E73" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2462,16 +2369,16 @@
       <c r="A74" s="17">
         <v>73</v>
       </c>
-      <c r="B74" s="26">
+      <c r="B74" s="14">
         <v>100</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D74" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E74" s="3">
+      <c r="D74" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E74" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2479,16 +2386,16 @@
       <c r="A75" s="17">
         <v>74</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E75" s="3">
+      <c r="D75" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E75" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2496,16 +2403,16 @@
       <c r="A76" s="17">
         <v>75</v>
       </c>
-      <c r="B76" s="26" t="s">
+      <c r="B76" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E76" s="3">
+      <c r="D76" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E76" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2513,16 +2420,16 @@
       <c r="A77" s="17">
         <v>76</v>
       </c>
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E77" s="3">
+      <c r="D77" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E77" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2530,16 +2437,16 @@
       <c r="A78" s="17">
         <v>77</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="B78" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D78" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E78" s="3">
+      <c r="D78" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E78" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2547,16 +2454,16 @@
       <c r="A79" s="17">
         <v>78</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E79" s="3">
+      <c r="D79" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E79" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2564,16 +2471,16 @@
       <c r="A80" s="17">
         <v>79</v>
       </c>
-      <c r="B80" s="26" t="s">
+      <c r="B80" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D80" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E80" s="3">
+      <c r="D80" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E80" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2581,16 +2488,16 @@
       <c r="A81" s="17">
         <v>80</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D81" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E81" s="3">
+      <c r="D81" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E81" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2598,16 +2505,16 @@
       <c r="A82" s="17">
         <v>81</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D82" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E82" s="3">
+      <c r="D82" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E82" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2615,16 +2522,16 @@
       <c r="A83" s="17">
         <v>82</v>
       </c>
-      <c r="B83" s="26" t="s">
+      <c r="B83" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C83" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E83" s="3">
+      <c r="D83" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E83" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2632,16 +2539,16 @@
       <c r="A84" s="17">
         <v>83</v>
       </c>
-      <c r="B84" s="26" t="s">
+      <c r="B84" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E84" s="3">
+      <c r="D84" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E84" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2649,16 +2556,16 @@
       <c r="A85" s="17">
         <v>84</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B85" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="21">
-        <v>1800</v>
-      </c>
-      <c r="E85" s="3">
+      <c r="D85" s="9">
+        <v>1800</v>
+      </c>
+      <c r="E85" s="9">
         <v>1800</v>
       </c>
     </row>
@@ -2666,16 +2573,16 @@
       <c r="A86" s="17">
         <v>85</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B86" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C86" s="25" t="s">
+      <c r="C86" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D86" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E86" s="3">
+      <c r="D86" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E86" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2683,16 +2590,16 @@
       <c r="A87" s="17">
         <v>86</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B87" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C87" s="25" t="s">
+      <c r="C87" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D87" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E87" s="3">
+      <c r="D87" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E87" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2700,16 +2607,16 @@
       <c r="A88" s="17">
         <v>87</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B88" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C88" s="25" t="s">
+      <c r="C88" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D88" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E88" s="3">
+      <c r="D88" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E88" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2717,16 +2624,16 @@
       <c r="A89" s="17">
         <v>88</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B89" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="25" t="s">
+      <c r="C89" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D89" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E89" s="3">
+      <c r="D89" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E89" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2734,16 +2641,16 @@
       <c r="A90" s="17">
         <v>89</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B90" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="25" t="s">
+      <c r="C90" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D90" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E90" s="3">
+      <c r="D90" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E90" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2751,16 +2658,16 @@
       <c r="A91" s="17">
         <v>90</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="25" t="s">
+      <c r="C91" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D91" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E91" s="3">
+      <c r="D91" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E91" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2768,16 +2675,16 @@
       <c r="A92" s="17">
         <v>91</v>
       </c>
-      <c r="B92" s="24" t="s">
+      <c r="B92" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C92" s="25" t="s">
+      <c r="C92" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D92" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E92" s="3">
+      <c r="D92" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E92" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2785,16 +2692,16 @@
       <c r="A93" s="17">
         <v>92</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="25" t="s">
+      <c r="C93" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D93" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E93" s="3">
+      <c r="D93" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E93" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2802,16 +2709,16 @@
       <c r="A94" s="17">
         <v>93</v>
       </c>
-      <c r="B94" s="24" t="s">
+      <c r="B94" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C94" s="25" t="s">
+      <c r="C94" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D94" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E94" s="3">
+      <c r="D94" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E94" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2819,16 +2726,16 @@
       <c r="A95" s="17">
         <v>94</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B95" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C95" s="25" t="s">
+      <c r="C95" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D95" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E95" s="3">
+      <c r="D95" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E95" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2836,16 +2743,16 @@
       <c r="A96" s="17">
         <v>95</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B96" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C96" s="25" t="s">
+      <c r="C96" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D96" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E96" s="3">
+      <c r="D96" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E96" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2853,16 +2760,16 @@
       <c r="A97" s="17">
         <v>96</v>
       </c>
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C97" s="23" t="s">
+      <c r="C97" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D97" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E97" s="3">
+      <c r="D97" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E97" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2870,16 +2777,16 @@
       <c r="A98" s="17">
         <v>97</v>
       </c>
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="23" t="s">
+      <c r="C98" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D98" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E98" s="3">
+      <c r="D98" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E98" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2887,16 +2794,16 @@
       <c r="A99" s="17">
         <v>98</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="C99" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D99" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E99" s="3">
+      <c r="D99" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E99" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2904,16 +2811,16 @@
       <c r="A100" s="17">
         <v>99</v>
       </c>
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D100" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E100" s="3">
+      <c r="D100" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E100" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2921,16 +2828,16 @@
       <c r="A101" s="17">
         <v>100</v>
       </c>
-      <c r="B101" s="22" t="s">
+      <c r="B101" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C101" s="23" t="s">
+      <c r="C101" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D101" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E101" s="3">
+      <c r="D101" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E101" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2938,16 +2845,16 @@
       <c r="A102" s="17">
         <v>101</v>
       </c>
-      <c r="B102" s="22" t="s">
+      <c r="B102" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C102" s="23" t="s">
+      <c r="C102" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D102" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E102" s="3">
+      <c r="D102" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E102" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2955,16 +2862,16 @@
       <c r="A103" s="17">
         <v>102</v>
       </c>
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C103" s="23" t="s">
+      <c r="C103" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D103" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E103" s="3">
+      <c r="D103" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E103" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2972,16 +2879,16 @@
       <c r="A104" s="17">
         <v>103</v>
       </c>
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C104" s="23" t="s">
+      <c r="C104" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D104" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E104" s="3">
+      <c r="D104" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E104" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -2989,16 +2896,16 @@
       <c r="A105" s="17">
         <v>104</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C105" s="23" t="s">
+      <c r="C105" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E105" s="3">
+      <c r="D105" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E105" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3006,16 +2913,16 @@
       <c r="A106" s="17">
         <v>105</v>
       </c>
-      <c r="B106" s="26" t="s">
+      <c r="B106" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D106" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E106" s="3">
+      <c r="D106" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E106" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3023,16 +2930,16 @@
       <c r="A107" s="17">
         <v>106</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D107" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E107" s="3">
+      <c r="D107" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E107" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3040,16 +2947,16 @@
       <c r="A108" s="17">
         <v>107</v>
       </c>
-      <c r="B108" s="26" t="s">
+      <c r="B108" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C108" s="20" t="s">
+      <c r="C108" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D108" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E108" s="3">
+      <c r="D108" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E108" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3057,16 +2964,16 @@
       <c r="A109" s="17">
         <v>108</v>
       </c>
-      <c r="B109" s="26" t="s">
+      <c r="B109" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C109" s="20" t="s">
+      <c r="C109" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D109" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E109" s="3">
+      <c r="D109" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E109" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3074,16 +2981,16 @@
       <c r="A110" s="17">
         <v>109</v>
       </c>
-      <c r="B110" s="26" t="s">
+      <c r="B110" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C110" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D110" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E110" s="3">
+      <c r="D110" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E110" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3091,16 +2998,16 @@
       <c r="A111" s="17">
         <v>110</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D111" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E111" s="3">
+      <c r="D111" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E111" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3108,16 +3015,16 @@
       <c r="A112" s="17">
         <v>111</v>
       </c>
-      <c r="B112" s="24" t="s">
+      <c r="B112" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C112" s="25" t="s">
+      <c r="C112" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D112" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E112" s="3">
+      <c r="D112" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E112" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3125,16 +3032,16 @@
       <c r="A113" s="17">
         <v>112</v>
       </c>
-      <c r="B113" s="24" t="s">
+      <c r="B113" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C113" s="25" t="s">
+      <c r="C113" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D113" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E113" s="3">
+      <c r="D113" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E113" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3142,16 +3049,16 @@
       <c r="A114" s="17">
         <v>113</v>
       </c>
-      <c r="B114" s="24" t="s">
+      <c r="B114" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C114" s="25" t="s">
+      <c r="C114" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D114" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E114" s="3">
+      <c r="D114" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E114" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3159,16 +3066,16 @@
       <c r="A115" s="17">
         <v>114</v>
       </c>
-      <c r="B115" s="24" t="s">
+      <c r="B115" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C115" s="25" t="s">
+      <c r="C115" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D115" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E115" s="3">
+      <c r="D115" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E115" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3176,16 +3083,16 @@
       <c r="A116" s="17">
         <v>115</v>
       </c>
-      <c r="B116" s="24" t="s">
+      <c r="B116" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C116" s="25" t="s">
+      <c r="C116" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D116" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E116" s="3">
+      <c r="D116" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E116" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3193,16 +3100,16 @@
       <c r="A117" s="17">
         <v>116</v>
       </c>
-      <c r="B117" s="27" t="s">
+      <c r="B117" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C117" s="28" t="s">
+      <c r="C117" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D117" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E117" s="3">
+      <c r="D117" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E117" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3210,16 +3117,16 @@
       <c r="A118" s="17">
         <v>117</v>
       </c>
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C118" s="28" t="s">
+      <c r="C118" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D118" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E118" s="3">
+      <c r="D118" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E118" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3227,16 +3134,16 @@
       <c r="A119" s="17">
         <v>118</v>
       </c>
-      <c r="B119" s="27" t="s">
+      <c r="B119" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C119" s="28" t="s">
+      <c r="C119" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D119" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E119" s="3">
+      <c r="D119" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E119" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3244,16 +3151,16 @@
       <c r="A120" s="17">
         <v>119</v>
       </c>
-      <c r="B120" s="27" t="s">
+      <c r="B120" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="C120" s="28" t="s">
+      <c r="C120" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D120" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E120" s="3">
+      <c r="D120" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E120" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3261,16 +3168,16 @@
       <c r="A121" s="17">
         <v>120</v>
       </c>
-      <c r="B121" s="27" t="s">
+      <c r="B121" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C121" s="28" t="s">
+      <c r="C121" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D121" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E121" s="3">
+      <c r="D121" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E121" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3278,16 +3185,16 @@
       <c r="A122" s="17">
         <v>121</v>
       </c>
-      <c r="B122" s="27" t="s">
+      <c r="B122" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C122" s="28" t="s">
+      <c r="C122" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D122" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E122" s="3">
+      <c r="D122" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E122" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3295,16 +3202,16 @@
       <c r="A123" s="17">
         <v>122</v>
       </c>
-      <c r="B123" s="27" t="s">
+      <c r="B123" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C123" s="28" t="s">
+      <c r="C123" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D123" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E123" s="3">
+      <c r="D123" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E123" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3312,16 +3219,16 @@
       <c r="A124" s="17">
         <v>123</v>
       </c>
-      <c r="B124" s="27" t="s">
+      <c r="B124" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C124" s="28" t="s">
+      <c r="C124" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D124" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E124" s="3">
+      <c r="D124" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E124" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3329,16 +3236,16 @@
       <c r="A125" s="17">
         <v>124</v>
       </c>
-      <c r="B125" s="26" t="s">
+      <c r="B125" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="20" t="s">
+      <c r="C125" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D125" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E125" s="3">
+      <c r="D125" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E125" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3346,16 +3253,16 @@
       <c r="A126" s="17">
         <v>125</v>
       </c>
-      <c r="B126" s="26" t="s">
+      <c r="B126" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="20" t="s">
+      <c r="C126" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D126" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E126" s="3">
+      <c r="D126" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E126" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3363,16 +3270,16 @@
       <c r="A127" s="17">
         <v>126</v>
       </c>
-      <c r="B127" s="26" t="s">
+      <c r="B127" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="20" t="s">
+      <c r="C127" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D127" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E127" s="3">
+      <c r="D127" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E127" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3380,16 +3287,16 @@
       <c r="A128" s="17">
         <v>127</v>
       </c>
-      <c r="B128" s="26" t="s">
+      <c r="B128" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C128" s="20" t="s">
+      <c r="C128" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D128" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E128" s="3">
+      <c r="D128" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E128" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3397,16 +3304,16 @@
       <c r="A129" s="17">
         <v>128</v>
       </c>
-      <c r="B129" s="26" t="s">
+      <c r="B129" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C129" s="20" t="s">
+      <c r="C129" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D129" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E129" s="3">
+      <c r="D129" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E129" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3414,16 +3321,16 @@
       <c r="A130" s="17">
         <v>129</v>
       </c>
-      <c r="B130" s="26" t="s">
+      <c r="B130" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="20" t="s">
+      <c r="C130" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D130" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E130" s="3">
+      <c r="D130" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E130" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3431,16 +3338,16 @@
       <c r="A131" s="17">
         <v>130</v>
       </c>
-      <c r="B131" s="26" t="s">
+      <c r="B131" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C131" s="20" t="s">
+      <c r="C131" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D131" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E131" s="3">
+      <c r="D131" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E131" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3448,16 +3355,16 @@
       <c r="A132" s="17">
         <v>131</v>
       </c>
-      <c r="B132" s="26" t="s">
+      <c r="B132" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C132" s="20" t="s">
+      <c r="C132" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D132" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E132" s="3">
+      <c r="D132" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E132" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3465,16 +3372,16 @@
       <c r="A133" s="17">
         <v>132</v>
       </c>
-      <c r="B133" s="26" t="s">
+      <c r="B133" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C133" s="20" t="s">
+      <c r="C133" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D133" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E133" s="3">
+      <c r="D133" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E133" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3482,16 +3389,16 @@
       <c r="A134" s="17">
         <v>133</v>
       </c>
-      <c r="B134" s="26" t="s">
+      <c r="B134" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C134" s="20" t="s">
+      <c r="C134" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D134" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E134" s="3">
+      <c r="D134" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E134" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3499,16 +3406,16 @@
       <c r="A135" s="17">
         <v>134</v>
       </c>
-      <c r="B135" s="26" t="s">
+      <c r="B135" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C135" s="20" t="s">
+      <c r="C135" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D135" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E135" s="3">
+      <c r="D135" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E135" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3516,16 +3423,16 @@
       <c r="A136" s="17">
         <v>135</v>
       </c>
-      <c r="B136" s="26" t="s">
+      <c r="B136" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C136" s="20" t="s">
+      <c r="C136" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D136" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E136" s="3">
+      <c r="D136" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E136" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3533,16 +3440,16 @@
       <c r="A137" s="17">
         <v>136</v>
       </c>
-      <c r="B137" s="26" t="s">
+      <c r="B137" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="C137" s="20" t="s">
+      <c r="C137" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D137" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E137" s="3">
+      <c r="D137" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E137" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3550,16 +3457,16 @@
       <c r="A138" s="17">
         <v>137</v>
       </c>
-      <c r="B138" s="24" t="s">
+      <c r="B138" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C138" s="25" t="s">
+      <c r="C138" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D138" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E138" s="3">
+      <c r="D138" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E138" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3567,16 +3474,16 @@
       <c r="A139" s="17">
         <v>138</v>
       </c>
-      <c r="B139" s="24" t="s">
+      <c r="B139" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C139" s="25" t="s">
+      <c r="C139" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D139" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E139" s="3">
+      <c r="D139" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E139" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3584,16 +3491,16 @@
       <c r="A140" s="17">
         <v>139</v>
       </c>
-      <c r="B140" s="24" t="s">
+      <c r="B140" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C140" s="25" t="s">
+      <c r="C140" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D140" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E140" s="3">
+      <c r="D140" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E140" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3601,16 +3508,16 @@
       <c r="A141" s="17">
         <v>140</v>
       </c>
-      <c r="B141" s="24" t="s">
+      <c r="B141" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C141" s="25" t="s">
+      <c r="C141" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D141" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E141" s="3">
+      <c r="D141" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E141" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3618,16 +3525,16 @@
       <c r="A142" s="17">
         <v>141</v>
       </c>
-      <c r="B142" s="24" t="s">
+      <c r="B142" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C142" s="25" t="s">
+      <c r="C142" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D142" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E142" s="3">
+      <c r="D142" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E142" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3635,16 +3542,16 @@
       <c r="A143" s="17">
         <v>142</v>
       </c>
-      <c r="B143" s="24" t="s">
+      <c r="B143" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C143" s="25" t="s">
+      <c r="C143" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D143" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E143" s="3">
+      <c r="D143" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E143" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3652,16 +3559,16 @@
       <c r="A144" s="17">
         <v>143</v>
       </c>
-      <c r="B144" s="24" t="s">
+      <c r="B144" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C144" s="25" t="s">
+      <c r="C144" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D144" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E144" s="3">
+      <c r="D144" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E144" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3669,16 +3576,16 @@
       <c r="A145" s="17">
         <v>144</v>
       </c>
-      <c r="B145" s="24" t="s">
+      <c r="B145" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C145" s="25" t="s">
+      <c r="C145" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D145" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E145" s="3">
+      <c r="D145" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E145" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3686,16 +3593,16 @@
       <c r="A146" s="17">
         <v>145</v>
       </c>
-      <c r="B146" s="24" t="s">
+      <c r="B146" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C146" s="25" t="s">
+      <c r="C146" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D146" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E146" s="3">
+      <c r="D146" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E146" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3703,16 +3610,16 @@
       <c r="A147" s="17">
         <v>146</v>
       </c>
-      <c r="B147" s="22" t="s">
+      <c r="B147" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C147" s="23" t="s">
+      <c r="C147" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D147" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E147" s="3">
+      <c r="D147" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E147" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3720,16 +3627,16 @@
       <c r="A148" s="17">
         <v>147</v>
       </c>
-      <c r="B148" s="22" t="s">
+      <c r="B148" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C148" s="23" t="s">
+      <c r="C148" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D148" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E148" s="3">
+      <c r="D148" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E148" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3737,16 +3644,16 @@
       <c r="A149" s="17">
         <v>148</v>
       </c>
-      <c r="B149" s="22" t="s">
+      <c r="B149" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C149" s="23" t="s">
+      <c r="C149" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D149" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E149" s="3">
+      <c r="D149" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E149" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3754,16 +3661,16 @@
       <c r="A150" s="17">
         <v>149</v>
       </c>
-      <c r="B150" s="22" t="s">
+      <c r="B150" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C150" s="23" t="s">
+      <c r="C150" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D150" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E150" s="3">
+      <c r="D150" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E150" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3771,16 +3678,16 @@
       <c r="A151" s="17">
         <v>150</v>
       </c>
-      <c r="B151" s="22" t="s">
+      <c r="B151" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C151" s="23" t="s">
+      <c r="C151" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D151" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E151" s="3">
+      <c r="D151" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E151" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3788,16 +3695,16 @@
       <c r="A152" s="17">
         <v>151</v>
       </c>
-      <c r="B152" s="22" t="s">
+      <c r="B152" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C152" s="23" t="s">
+      <c r="C152" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D152" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E152" s="3">
+      <c r="D152" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E152" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3805,16 +3712,16 @@
       <c r="A153" s="17">
         <v>152</v>
       </c>
-      <c r="B153" s="22" t="s">
+      <c r="B153" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C153" s="23" t="s">
+      <c r="C153" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D153" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E153" s="3">
+      <c r="D153" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E153" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3822,16 +3729,16 @@
       <c r="A154" s="17">
         <v>153</v>
       </c>
-      <c r="B154" s="22" t="s">
+      <c r="B154" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C154" s="23" t="s">
+      <c r="C154" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D154" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E154" s="3">
+      <c r="D154" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E154" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3839,16 +3746,16 @@
       <c r="A155" s="17">
         <v>154</v>
       </c>
-      <c r="B155" s="22" t="s">
+      <c r="B155" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C155" s="23" t="s">
+      <c r="C155" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D155" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E155" s="3">
+      <c r="D155" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E155" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3856,16 +3763,16 @@
       <c r="A156" s="17">
         <v>155</v>
       </c>
-      <c r="B156" s="22" t="s">
+      <c r="B156" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C156" s="23" t="s">
+      <c r="C156" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D156" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E156" s="3">
+      <c r="D156" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E156" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3873,16 +3780,16 @@
       <c r="A157" s="17">
         <v>156</v>
       </c>
-      <c r="B157" s="22" t="s">
+      <c r="B157" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C157" s="23" t="s">
+      <c r="C157" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D157" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E157" s="3">
+      <c r="D157" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E157" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3890,16 +3797,16 @@
       <c r="A158" s="17">
         <v>157</v>
       </c>
-      <c r="B158" s="22" t="s">
+      <c r="B158" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C158" s="23" t="s">
+      <c r="C158" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D158" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E158" s="3">
+      <c r="D158" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E158" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3907,16 +3814,16 @@
       <c r="A159" s="17">
         <v>158</v>
       </c>
-      <c r="B159" s="22" t="s">
+      <c r="B159" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C159" s="23" t="s">
+      <c r="C159" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D159" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E159" s="3">
+      <c r="D159" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E159" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3924,16 +3831,16 @@
       <c r="A160" s="17">
         <v>159</v>
       </c>
-      <c r="B160" s="22" t="s">
+      <c r="B160" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="C160" s="23" t="s">
+      <c r="C160" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D160" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E160" s="3">
+      <c r="D160" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E160" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3941,16 +3848,16 @@
       <c r="A161" s="17">
         <v>160</v>
       </c>
-      <c r="B161" s="22" t="s">
+      <c r="B161" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C161" s="23" t="s">
+      <c r="C161" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D161" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E161" s="3">
+      <c r="D161" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E161" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3958,16 +3865,16 @@
       <c r="A162" s="17">
         <v>161</v>
       </c>
-      <c r="B162" s="26" t="s">
+      <c r="B162" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C162" s="20" t="s">
+      <c r="C162" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D162" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E162" s="3">
+      <c r="D162" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E162" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3975,16 +3882,16 @@
       <c r="A163" s="17">
         <v>162</v>
       </c>
-      <c r="B163" s="26" t="s">
+      <c r="B163" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C163" s="20" t="s">
+      <c r="C163" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D163" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E163" s="3">
+      <c r="D163" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E163" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -3992,16 +3899,16 @@
       <c r="A164" s="17">
         <v>163</v>
       </c>
-      <c r="B164" s="26" t="s">
+      <c r="B164" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C164" s="20" t="s">
+      <c r="C164" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D164" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E164" s="3">
+      <c r="D164" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E164" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4009,16 +3916,16 @@
       <c r="A165" s="17">
         <v>164</v>
       </c>
-      <c r="B165" s="26" t="s">
+      <c r="B165" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C165" s="20" t="s">
+      <c r="C165" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D165" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E165" s="3">
+      <c r="D165" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E165" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4026,16 +3933,16 @@
       <c r="A166" s="17">
         <v>165</v>
       </c>
-      <c r="B166" s="26" t="s">
+      <c r="B166" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C166" s="20" t="s">
+      <c r="C166" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D166" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E166" s="3">
+      <c r="D166" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E166" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4043,16 +3950,16 @@
       <c r="A167" s="17">
         <v>166</v>
       </c>
-      <c r="B167" s="26" t="s">
+      <c r="B167" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C167" s="20" t="s">
+      <c r="C167" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D167" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E167" s="3">
+      <c r="D167" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E167" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4060,16 +3967,16 @@
       <c r="A168" s="17">
         <v>167</v>
       </c>
-      <c r="B168" s="26" t="s">
+      <c r="B168" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C168" s="20" t="s">
+      <c r="C168" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D168" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E168" s="3">
+      <c r="D168" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E168" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4077,16 +3984,16 @@
       <c r="A169" s="17">
         <v>168</v>
       </c>
-      <c r="B169" s="26" t="s">
+      <c r="B169" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C169" s="20" t="s">
+      <c r="C169" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D169" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E169" s="3">
+      <c r="D169" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E169" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4094,16 +4001,16 @@
       <c r="A170" s="17">
         <v>169</v>
       </c>
-      <c r="B170" s="26" t="s">
+      <c r="B170" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C170" s="20" t="s">
+      <c r="C170" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D170" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E170" s="3">
+      <c r="D170" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E170" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4111,16 +4018,16 @@
       <c r="A171" s="17">
         <v>170</v>
       </c>
-      <c r="B171" s="26" t="s">
+      <c r="B171" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C171" s="20" t="s">
+      <c r="C171" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D171" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E171" s="3">
+      <c r="D171" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E171" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4128,16 +4035,16 @@
       <c r="A172" s="17">
         <v>171</v>
       </c>
-      <c r="B172" s="26" t="s">
+      <c r="B172" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C172" s="20" t="s">
+      <c r="C172" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D172" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E172" s="3">
+      <c r="D172" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E172" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4145,16 +4052,16 @@
       <c r="A173" s="17">
         <v>172</v>
       </c>
-      <c r="B173" s="26" t="s">
+      <c r="B173" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C173" s="20" t="s">
+      <c r="C173" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D173" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E173" s="3">
+      <c r="D173" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E173" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4162,16 +4069,16 @@
       <c r="A174" s="17">
         <v>173</v>
       </c>
-      <c r="B174" s="24" t="s">
+      <c r="B174" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C174" s="25" t="s">
+      <c r="C174" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D174" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E174" s="3">
+      <c r="D174" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E174" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4179,16 +4086,16 @@
       <c r="A175" s="17">
         <v>174</v>
       </c>
-      <c r="B175" s="24" t="s">
+      <c r="B175" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C175" s="25" t="s">
+      <c r="C175" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D175" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E175" s="3">
+      <c r="D175" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E175" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4196,16 +4103,16 @@
       <c r="A176" s="17">
         <v>175</v>
       </c>
-      <c r="B176" s="24" t="s">
+      <c r="B176" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C176" s="25" t="s">
+      <c r="C176" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D176" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E176" s="3">
+      <c r="D176" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E176" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4213,16 +4120,16 @@
       <c r="A177" s="17">
         <v>176</v>
       </c>
-      <c r="B177" s="24" t="s">
+      <c r="B177" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C177" s="25" t="s">
+      <c r="C177" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D177" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E177" s="3">
+      <c r="D177" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E177" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4230,16 +4137,16 @@
       <c r="A178" s="17">
         <v>177</v>
       </c>
-      <c r="B178" s="24" t="s">
+      <c r="B178" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C178" s="25" t="s">
+      <c r="C178" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D178" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E178" s="3">
+      <c r="D178" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E178" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4247,16 +4154,16 @@
       <c r="A179" s="17">
         <v>178</v>
       </c>
-      <c r="B179" s="24" t="s">
+      <c r="B179" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C179" s="25" t="s">
+      <c r="C179" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D179" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E179" s="3">
+      <c r="D179" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E179" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4264,16 +4171,16 @@
       <c r="A180" s="17">
         <v>179</v>
       </c>
-      <c r="B180" s="24" t="s">
+      <c r="B180" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C180" s="25" t="s">
+      <c r="C180" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D180" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E180" s="3">
+      <c r="D180" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E180" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4281,16 +4188,16 @@
       <c r="A181" s="17">
         <v>180</v>
       </c>
-      <c r="B181" s="24" t="s">
+      <c r="B181" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C181" s="25" t="s">
+      <c r="C181" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D181" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E181" s="3">
+      <c r="D181" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E181" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4298,16 +4205,16 @@
       <c r="A182" s="17">
         <v>181</v>
       </c>
-      <c r="B182" s="24" t="s">
+      <c r="B182" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C182" s="25" t="s">
+      <c r="C182" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D182" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E182" s="3">
+      <c r="D182" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E182" s="9">
         <v>1650</v>
       </c>
     </row>
@@ -4315,38 +4222,35 @@
       <c r="A183" s="17">
         <v>182</v>
       </c>
-      <c r="B183" s="24" t="s">
+      <c r="B183" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C183" s="25" t="s">
+      <c r="C183" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D183" s="21">
-        <v>1650</v>
-      </c>
-      <c r="E183" s="3">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A184" s="18">
+      <c r="D183" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E183" s="9">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="17">
         <v>183</v>
       </c>
-      <c r="B184" s="14" t="s">
+      <c r="B184" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C184" s="15" t="s">
+      <c r="C184" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D184" s="2">
-        <v>1650</v>
-      </c>
-      <c r="E184" s="4">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A185"/>
+      <c r="D184" s="9">
+        <v>1650</v>
+      </c>
+      <c r="E184" s="9">
+        <v>1650</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186"/>

</xml_diff>